<commit_message>
actualización video 12 esperas explicitas
</commit_message>
<xml_diff>
--- a/src/main/java/Recursos/Data/Insumos/copia/Testing.xlsx
+++ b/src/main/java/Recursos/Data/Insumos/copia/Testing.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\SeleniumJavaDesde0\src\main\java\Recursos\Data\Insumos\copia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\SeleniumJavaDesde0\src\main\java\Recursos\Data\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E265A84-29A1-47A4-865F-538840306719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E92DB-9B1B-4130-889C-EE520FEE92E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="6630" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="5835" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
   <si>
     <t>usuario</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>resultado</t>
+  </si>
+  <si>
+    <t>fallo</t>
   </si>
   <si>
     <t>ok</t>
@@ -109,6 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,19 +455,19 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -498,11 +502,11 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
+      <c r="B2" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -536,8 +540,11 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -571,8 +578,11 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
@@ -606,8 +616,11 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
@@ -641,8 +654,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>20</v>
@@ -676,8 +692,11 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>21</v>

</xml_diff>